<commit_message>
bug fix - valid space
</commit_message>
<xml_diff>
--- a/data/preprocessed_data/df_preprocessed.xlsx
+++ b/data/preprocessed_data/df_preprocessed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q617269\Desktop\Masterarbeit_Tobias\repos\master-thesis\data\preprocessed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A062D-E2CF-4F07-8268-105A0CDE1BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17310EAB-426C-41EE-8B94-20FAD6A29FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="39">
   <si>
     <t>Relevant fuer Messung</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Z-Max_transf</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
   <si>
     <t>DICHTUNG HECKKLAPPE</t>
@@ -538,15 +541,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:J165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A2" sqref="A2:XFD4087"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,16 +574,19 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>1284.4698490000001</v>
@@ -600,16 +606,19 @@
       <c r="I2">
         <v>1030.0268550000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>3116867419.8635159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>764.02868699999999</v>
@@ -629,16 +638,19 @@
       <c r="I3">
         <v>717.01409899999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>12286387.26057039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>285</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>3233.7651369999999</v>
@@ -658,16 +670,19 @@
       <c r="I4">
         <v>722.24963400000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>287956071.11179131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>292</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>3347.358154</v>
@@ -687,16 +702,19 @@
       <c r="I5">
         <v>708.08502199999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>133447286.8565042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>304</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>3179.3222660000001</v>
@@ -716,16 +734,19 @@
       <c r="I6">
         <v>198.03796399999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>377079640.54395348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>314</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>3671.6457519999999</v>
@@ -745,16 +766,19 @@
       <c r="I7">
         <v>679.94885299999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>4395391.1287168721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>315</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>467.51364100000001</v>
@@ -774,16 +798,19 @@
       <c r="I8">
         <v>973.816284</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>460341926.85456371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>399</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>1273.6376949999999</v>
@@ -803,16 +830,19 @@
       <c r="I9">
         <v>934.96313499999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>3005053.9451211751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>400</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1273.6376949999999</v>
@@ -832,16 +862,19 @@
       <c r="I10">
         <v>934.96313499999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>3005053.9451211751</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>401</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>703.96423300000004</v>
@@ -861,16 +894,19 @@
       <c r="I11">
         <v>902.18194600000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>29217989.5041558</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>406</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>620.42156999999997</v>
@@ -890,16 +926,19 @@
       <c r="I12">
         <v>309.13751200000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>7778674.0579851121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>448</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13">
         <v>2475.5122070000002</v>
@@ -919,16 +958,19 @@
       <c r="I13">
         <v>222.32635500000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>70853517.605508074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>449</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>2484.8005370000001</v>
@@ -948,16 +990,19 @@
       <c r="I14">
         <v>670.04663100000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>270554250.13993752</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>452</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>3536.8139649999998</v>
@@ -977,16 +1022,19 @@
       <c r="I15">
         <v>404.66760299999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>24197285.633770879</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>700</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16">
         <v>1224.3739009999999</v>
@@ -1006,16 +1054,19 @@
       <c r="I16">
         <v>1031.113525</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>190151379.48631811</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>779</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>764.02868699999999</v>
@@ -1035,16 +1086,19 @@
       <c r="I17">
         <v>717.01409899999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>12286387.26057039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>830</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>746.51446499999997</v>
@@ -1064,16 +1118,19 @@
       <c r="I18">
         <v>934.05706799999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>207108548.56353459</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>843</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>3171.7233890000002</v>
@@ -1093,16 +1150,19 @@
       <c r="I19">
         <v>736.793091</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>333926592.1432296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>851</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <v>3257.8571780000002</v>
@@ -1122,16 +1182,19 @@
       <c r="I20">
         <v>714.339111</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>172579455.72286719</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>863</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>3179.3222660000001</v>
@@ -1151,16 +1214,19 @@
       <c r="I21">
         <v>198.03796399999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>377079640.54395348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>872</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>2393.2126459999999</v>
@@ -1180,16 +1246,19 @@
       <c r="I22">
         <v>943.86700399999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>2861444.451779569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>874</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>467.51364100000001</v>
@@ -1209,16 +1278,19 @@
       <c r="I23">
         <v>973.816284</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>460341926.85456371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>875</v>
       </c>
       <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
         <v>12</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
       </c>
       <c r="D24">
         <v>2383.531982</v>
@@ -1238,16 +1310,19 @@
       <c r="I24">
         <v>952.06408699999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>262488333.85280579</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>940</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25">
         <v>1295.355591</v>
@@ -1267,16 +1342,19 @@
       <c r="I25">
         <v>943.24816899999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>2605736.7509720302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>941</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>705.11157200000002</v>
@@ -1296,16 +1374,19 @@
       <c r="I26">
         <v>904.68487500000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>31181455.210011311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>945</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>1195.968384</v>
@@ -1325,16 +1406,19 @@
       <c r="I27">
         <v>1024.8469239999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <v>533956456.56468308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>947</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28">
         <v>2299.8659670000002</v>
@@ -1354,16 +1438,19 @@
       <c r="I28">
         <v>944.64312700000005</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J28">
+        <v>2917773.1389583428</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>949</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29">
         <v>620.42138699999998</v>
@@ -1383,16 +1470,19 @@
       <c r="I29">
         <v>309.13751200000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>7760019.7748016911</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>994</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D30">
         <v>2475.420654</v>
@@ -1412,16 +1502,19 @@
       <c r="I30">
         <v>227.43670700000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J30">
+        <v>75628347.865811318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>995</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D31">
         <v>2458.814453</v>
@@ -1441,16 +1534,19 @@
       <c r="I31">
         <v>656.20001200000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <v>188608651.60712871</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>997</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D32">
         <v>3536.8139649999998</v>
@@ -1470,16 +1566,19 @@
       <c r="I32">
         <v>404.66760299999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J32">
+        <v>24197285.633770879</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1098</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>1032.1421930684801</v>
@@ -1499,16 +1598,19 @@
       <c r="I33">
         <v>928.59187415736119</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J33">
+        <v>6662053.7555670291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1300</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>1248.5908199999999</v>
@@ -1528,16 +1630,19 @@
       <c r="I34">
         <v>1080.8266599999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J34">
+        <v>3308752118.5323648</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1336</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35">
         <v>775.06494099999998</v>
@@ -1557,16 +1662,19 @@
       <c r="I35">
         <v>748.807007</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J35">
+        <v>21358983.239237592</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1393</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>3334.7292480000001</v>
@@ -1586,16 +1694,19 @@
       <c r="I36">
         <v>728.282104</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J36">
+        <v>304351430.39889699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1398</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D37">
         <v>3425.5783689999998</v>
@@ -1615,16 +1726,19 @@
       <c r="I37">
         <v>716.05938700000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37">
+        <v>141943383.915791</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1408</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>3488.8215329999998</v>
@@ -1644,16 +1758,19 @@
       <c r="I38">
         <v>129.99946600000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38">
+        <v>106813908.8100172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1416</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D39">
         <v>3721.7473140000002</v>
@@ -1673,16 +1790,19 @@
       <c r="I39">
         <v>707.47412099999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39">
+        <v>1663192.237470553</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1485</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D40">
         <v>1210.8835449999999</v>
@@ -1702,16 +1822,19 @@
       <c r="I40">
         <v>977.75579800000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40">
+        <v>4103728.501684946</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1486</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D41">
         <v>686.57421899999997</v>
@@ -1731,16 +1854,19 @@
       <c r="I41">
         <v>937.82586700000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J41">
+        <v>31133912.31276805</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1489</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D42">
         <v>591.49408000000005</v>
@@ -1760,16 +1886,19 @@
       <c r="I42">
         <v>279.671448</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J42">
+        <v>6234212.0570974071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1525</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D43">
         <v>2762.5344239999999</v>
@@ -1789,16 +1918,19 @@
       <c r="I43">
         <v>207.36158800000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J43">
+        <v>28665715.39918004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1527</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D44">
         <v>2770.75</v>
@@ -1818,16 +1950,19 @@
       <c r="I44">
         <v>670.03686500000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J44">
+        <v>158155300.7097275</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>1532</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D45">
         <v>3571.4726559999999</v>
@@ -1847,16 +1982,19 @@
       <c r="I45">
         <v>351.96475199999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J45">
+        <v>23444983.158251811</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>1632</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>1016.0481813022</v>
@@ -1876,16 +2014,19 @@
       <c r="I46">
         <v>970.06581382012951</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J46">
+        <v>4929621.1115717953</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>1773</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D47">
         <v>1200.225586</v>
@@ -1905,16 +2046,19 @@
       <c r="I47">
         <v>1153.5219729999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J47">
+        <v>401903963.47719991</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1864</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>698.64263900000003</v>
@@ -1934,16 +2078,19 @@
       <c r="I48">
         <v>762.58074999999997</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J48">
+        <v>21151233.43516472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1908</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D49">
         <v>731.720642</v>
@@ -1963,16 +2110,19 @@
       <c r="I49">
         <v>1016.175781</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J49">
+        <v>222806223.4113988</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>1909</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D50">
         <v>1799.6610109999999</v>
@@ -1992,16 +2142,19 @@
       <c r="I50">
         <v>1028.9985349999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J50">
+        <v>224542997.25596669</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>1925</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D51">
         <v>634.96557600000006</v>
@@ -2021,16 +2174,19 @@
       <c r="I51">
         <v>1069.948975</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J51">
+        <v>303747215.79968822</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>1940</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>3754.6860350000002</v>
@@ -2050,16 +2206,19 @@
       <c r="I52">
         <v>788.49352999999996</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J52">
+        <v>92183437.884501725</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1959</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D53">
         <v>3330.8916020000001</v>
@@ -2079,16 +2238,19 @@
       <c r="I53">
         <v>1069.6881100000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J53">
+        <v>575403670.1906333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1961</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D54">
         <v>3299.969482</v>
@@ -2108,16 +2270,19 @@
       <c r="I54">
         <v>1080.5830080000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J54">
+        <v>46058035.791716702</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1977</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D55">
         <v>3571.5780159379879</v>
@@ -2137,16 +2302,19 @@
       <c r="I55">
         <v>1011.094796183888</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J55">
+        <v>995518.69829942635</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1978</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D56">
         <v>463.17520100000002</v>
@@ -2166,16 +2334,19 @@
       <c r="I56">
         <v>1050.1719969999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J56">
+        <v>573162146.54022479</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1979</v>
       </c>
       <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
         <v>12</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
       </c>
       <c r="D57">
         <v>3421.4555660000001</v>
@@ -2195,16 +2366,19 @@
       <c r="I57">
         <v>994.23272699999995</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J57">
+        <v>180270454.24290681</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2038</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D58">
         <v>2756.824803</v>
@@ -2224,16 +2398,19 @@
       <c r="I58">
         <v>833.40449799999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J58">
+        <v>6776060.7104884097</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2070</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D59">
         <v>1275.6613769999999</v>
@@ -2253,16 +2430,19 @@
       <c r="I59">
         <v>1030.8093260000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J59">
+        <v>4488384.5768924421</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>2071</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D60">
         <v>1461.009033</v>
@@ -2282,16 +2462,19 @@
       <c r="I60">
         <v>1081.802124</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J60">
+        <v>1392925.6835431389</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>2074</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D61">
         <v>2288.0373540000001</v>
@@ -2311,16 +2494,19 @@
       <c r="I61">
         <v>1098.807251</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J61">
+        <v>1735465.935423509</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>2076</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D62">
         <v>673.40228300000001</v>
@@ -2340,16 +2526,19 @@
       <c r="I62">
         <v>988.89666699999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J62">
+        <v>35329731.61328961</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>2080</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D63">
         <v>1163.3607179999999</v>
@@ -2369,16 +2558,19 @@
       <c r="I63">
         <v>1156.173828</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J63">
+        <v>771034612.65438604</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>2081</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D64">
         <v>611.24334699999997</v>
@@ -2398,16 +2590,19 @@
       <c r="I64">
         <v>310.949005</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J64">
+        <v>22332724.49274718</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>2085</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D65">
         <v>1912.0001219999999</v>
@@ -2427,16 +2622,19 @@
       <c r="I65">
         <v>217.24269100000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J65">
+        <v>18854542.713296209</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>2110</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D66">
         <v>2730.5</v>
@@ -2456,16 +2654,19 @@
       <c r="I66">
         <v>311</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J66">
+        <v>60345431.267341457</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>2114</v>
       </c>
       <c r="B67" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D67">
         <v>2710.96875</v>
@@ -2485,16 +2686,19 @@
       <c r="I67">
         <v>716.31402600000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J67">
+        <v>177435737.996445</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2116</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D68">
         <v>3736.3413089999999</v>
@@ -2514,16 +2718,19 @@
       <c r="I68">
         <v>304</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J68">
+        <v>9293227.648824852</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2152</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D69">
         <v>742.29998799999998</v>
@@ -2543,16 +2750,19 @@
       <c r="I69">
         <v>640.17431599999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J69">
+        <v>1655607.6914827011</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>2195</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D70">
         <v>1848.31897</v>
@@ -2572,16 +2782,19 @@
       <c r="I70">
         <v>1038.571899</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J70">
+        <v>121156543.33588611</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>2215</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D71">
         <v>731.82202099999995</v>
@@ -2601,16 +2814,19 @@
       <c r="I71">
         <v>1026.354736</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J71">
+        <v>134824515.9012163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>2264</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D72">
         <v>993.5291373004294</v>
@@ -2630,16 +2846,19 @@
       <c r="I72">
         <v>1001.2421344836411</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J72">
+        <v>8041068.4114933386</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>2267</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D73">
         <v>2894.0655660420598</v>
@@ -2659,16 +2878,19 @@
       <c r="I73">
         <v>1163.780379597212</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J73">
+        <v>1788924.163083768</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>2268</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D74">
         <v>2899.9872467291761</v>
@@ -2688,16 +2910,19 @@
       <c r="I74">
         <v>1132.3018047673061</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J74">
+        <v>502801.10472188448</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>2399</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D75">
         <v>3012.7504880000001</v>
@@ -2717,16 +2942,19 @@
       <c r="I75">
         <v>1254.3145750000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J75">
+        <v>39937537.631623253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>2455</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D76">
         <v>1117.5115969999999</v>
@@ -2746,16 +2974,19 @@
       <c r="I76">
         <v>1317.462524</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J76">
+        <v>371403503.76864201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>2499</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D77">
         <v>672.14996299999996</v>
@@ -2775,16 +3006,19 @@
       <c r="I77">
         <v>911.44164999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J77">
+        <v>22362241.181072552</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>2525</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D78">
         <v>708.03802499999995</v>
@@ -2804,16 +3038,19 @@
       <c r="I78">
         <v>1189.1983640000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J78">
+        <v>235212960.05552709</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>2544</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D79">
         <v>634.05285600000002</v>
@@ -2833,16 +3070,19 @@
       <c r="I79">
         <v>1238.881836</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J79">
+        <v>293994355.63744599</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>2570</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D80">
         <v>3296.3869629999999</v>
@@ -2862,16 +3102,19 @@
       <c r="I80">
         <v>1227.4106449999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J80">
+        <v>39858456.13622795</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>2571</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D81">
         <v>3309.8271479999999</v>
@@ -2891,16 +3134,19 @@
       <c r="I81">
         <v>1213.5306399999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J81">
+        <v>663872194.80202699</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>2574</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D82">
         <v>3412.8576659999999</v>
@@ -2920,16 +3166,19 @@
       <c r="I82">
         <v>252.221161</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J82">
+        <v>484270405.14201868</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>2587</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D83">
         <v>3574.2370609999998</v>
@@ -2949,16 +3198,19 @@
       <c r="I83">
         <v>1153.517578</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J83">
+        <v>1005639.710654537</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>2588</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D84">
         <v>351.95764200000002</v>
@@ -2978,16 +3230,19 @@
       <c r="I84">
         <v>1191.970581</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J84">
+        <v>646682464.48011625</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>2589</v>
       </c>
       <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" t="s">
         <v>12</v>
-      </c>
-      <c r="C85" t="s">
-        <v>11</v>
       </c>
       <c r="D85">
         <v>3440.4560550000001</v>
@@ -3007,16 +3262,19 @@
       <c r="I85">
         <v>1134.9613039999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J85">
+        <v>184541291.3104502</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>2638</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D86">
         <v>2776.7905270000001</v>
@@ -3036,16 +3294,19 @@
       <c r="I86">
         <v>971.38653599999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J86">
+        <v>8558267.4259310309</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>2665</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D87">
         <v>1391.546509</v>
@@ -3065,16 +3326,19 @@
       <c r="I87">
         <v>1249.674438</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J87">
+        <v>1893027.3603401461</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>2668</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D88">
         <v>2217.6152339999999</v>
@@ -3094,16 +3358,19 @@
       <c r="I88">
         <v>1259.8579099999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J88">
+        <v>1773577.166692896</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>2670</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D89">
         <v>524.12091099999998</v>
@@ -3123,16 +3390,19 @@
       <c r="I89">
         <v>1123.9014890000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J89">
+        <v>35306845.062677547</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>2673</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D90">
         <v>1075.7342530000001</v>
@@ -3152,16 +3422,19 @@
       <c r="I90">
         <v>1257.1982419999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J90">
+        <v>750528201.86815631</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>2676</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D91">
         <v>1160.478801970406</v>
@@ -3181,16 +3454,19 @@
       <c r="I91">
         <v>1228.542216573775</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J91">
+        <v>12548810.728767401</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>2677</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D92">
         <v>496.5</v>
@@ -3210,16 +3486,19 @@
       <c r="I92">
         <v>353</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J92">
+        <v>40388034.09709233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>2681</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D93">
         <v>1970.947144</v>
@@ -3239,16 +3518,19 @@
       <c r="I93">
         <v>304.71447799999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J93">
+        <v>21163565.08271651</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>2713</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D94">
         <v>2733.154297</v>
@@ -3268,16 +3550,19 @@
       <c r="I94">
         <v>792.33862299999998</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J94">
+        <v>528223735.99014068</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>2715</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D95">
         <v>2659.313232</v>
@@ -3297,16 +3582,19 @@
       <c r="I95">
         <v>829.60003700000004</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95">
+        <v>188246074.5602878</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>2716</v>
       </c>
       <c r="B96" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D96">
         <v>3726.1496579999998</v>
@@ -3326,16 +3614,19 @@
       <c r="I96">
         <v>380.25082400000002</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J96">
+        <v>19960114.04006717</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>2738</v>
       </c>
       <c r="B97" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D97">
         <v>690.65142800000001</v>
@@ -3355,16 +3646,19 @@
       <c r="I97">
         <v>765.86291500000004</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J97">
+        <v>5491812.4317981647</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>2787</v>
       </c>
       <c r="B98" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D98">
         <v>1853.1697999999999</v>
@@ -3384,16 +3678,19 @@
       <c r="I98">
         <v>1207.4536129999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J98">
+        <v>130158596.4370307</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>2806</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D99">
         <v>707.95989999999995</v>
@@ -3413,16 +3710,19 @@
       <c r="I99">
         <v>1197.21875</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J99">
+        <v>121300707.7582356</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>2857</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D100">
         <v>909.42749543838124</v>
@@ -3442,16 +3742,19 @@
       <c r="I100">
         <v>1136.9026583524101</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J100">
+        <v>7385317.1001000712</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>2982</v>
       </c>
       <c r="B101" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D101">
         <v>2411.57251</v>
@@ -3471,16 +3774,19 @@
       <c r="I101">
         <v>1213.5054929999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J101">
+        <v>112425202.7303035</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>3035</v>
       </c>
       <c r="B102" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D102">
         <v>1068.665894</v>
@@ -3500,16 +3806,19 @@
       <c r="I102">
         <v>1231.648193</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J102">
+        <v>263156444.7873379</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>3063</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C103" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D103">
         <v>619.15429700000004</v>
@@ -3529,16 +3838,19 @@
       <c r="I103">
         <v>829.02099599999997</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J103">
+        <v>12845468.493239909</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>3098</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D104">
         <v>644.83227499999998</v>
@@ -3558,16 +3870,19 @@
       <c r="I104">
         <v>1090.259888</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J104">
+        <v>223885729.01405829</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>3099</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C105" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D105">
         <v>1685.0317379999999</v>
@@ -3587,16 +3902,19 @@
       <c r="I105">
         <v>1103.559082</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J105">
+        <v>212292401.0615741</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>3112</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C106" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D106">
         <v>512.74877900000001</v>
@@ -3616,16 +3934,19 @@
       <c r="I106">
         <v>1143.8454589999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J106">
+        <v>278851087.69414783</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>3125</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D107">
         <v>3183.3344729999999</v>
@@ -3645,16 +3966,19 @@
       <c r="I107">
         <v>1126.963745</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J107">
+        <v>436881020.73227191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>3143</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C108" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D108">
         <v>3151.5478520000001</v>
@@ -3674,16 +3998,19 @@
       <c r="I108">
         <v>1144.397217</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J108">
+        <v>75781424.474848121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>3144</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C109" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D109">
         <v>3169.6032709999999</v>
@@ -3703,16 +4030,19 @@
       <c r="I109">
         <v>1129.8206789999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J109">
+        <v>544690634.14361703</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>3151</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C110" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D110">
         <v>3564.0466310000002</v>
@@ -3732,16 +4062,19 @@
       <c r="I110">
         <v>169.67408800000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J110">
+        <v>120543018.34000351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>3158</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D111">
         <v>3496.720625925705</v>
@@ -3761,16 +4094,19 @@
       <c r="I111">
         <v>1059.4073233718</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J111">
+        <v>995504.56402691628</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>3159</v>
       </c>
       <c r="B112" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D112">
         <v>168.79808</v>
@@ -3790,16 +4126,19 @@
       <c r="I112">
         <v>1114.723389</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J112">
+        <v>743385241.11292827</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>3160</v>
       </c>
       <c r="B113" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" t="s">
         <v>12</v>
-      </c>
-      <c r="C113" t="s">
-        <v>11</v>
       </c>
       <c r="D113">
         <v>3304.1704100000002</v>
@@ -3819,16 +4158,19 @@
       <c r="I113">
         <v>1046.9873050000001</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J113">
+        <v>151156203.30609179</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>3206</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C114" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D114">
         <v>2624.0559079999998</v>
@@ -3848,16 +4190,19 @@
       <c r="I114">
         <v>897.31274399999995</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J114">
+        <v>12987533.297290999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>3238</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D115">
         <v>1129.0361330000001</v>
@@ -3877,16 +4222,19 @@
       <c r="I115">
         <v>1105.392456</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J115">
+        <v>4383993.8856919464</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>3240</v>
       </c>
       <c r="B116" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D116">
         <v>359.66861</v>
@@ -3906,16 +4254,19 @@
       <c r="I116">
         <v>1054.41626</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J116">
+        <v>46875677.065853037</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>3244</v>
       </c>
       <c r="B117" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D117">
         <v>1035.9426269999999</v>
@@ -3935,16 +4286,19 @@
       <c r="I117">
         <v>1208.130005</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J117">
+        <v>764153626.45658159</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>3247</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C118" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D118">
         <v>426.67022700000001</v>
@@ -3964,16 +4318,19 @@
       <c r="I118">
         <v>366</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J118">
+        <v>51057387.043277957</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>3256</v>
       </c>
       <c r="B119" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D119">
         <v>1857.8432620000001</v>
@@ -3993,16 +4350,19 @@
       <c r="I119">
         <v>363.28997800000002</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J119">
+        <v>72584427.855768412</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>3282</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C120" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D120">
         <v>2613.7065429999998</v>
@@ -4022,16 +4382,19 @@
       <c r="I120">
         <v>347.76788299999998</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J120">
+        <v>80908233.498167738</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>3284</v>
       </c>
       <c r="B121" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C121" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D121">
         <v>2634.5</v>
@@ -4051,16 +4414,19 @@
       <c r="I121">
         <v>710.66699200000005</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J121">
+        <v>156614795.32033539</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>3285</v>
       </c>
       <c r="B122" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C122" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D122">
         <v>3573.4936520000001</v>
@@ -4080,16 +4446,19 @@
       <c r="I122">
         <v>360.55062900000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J122">
+        <v>19763764.451679971</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>3311</v>
       </c>
       <c r="B123" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C123" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D123">
         <v>641</v>
@@ -4109,16 +4478,19 @@
       <c r="I123">
         <v>682.16711399999997</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J123">
+        <v>1536995.6537733199</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>3345</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C124" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D124">
         <v>1720.8496090000001</v>
@@ -4138,16 +4510,19 @@
       <c r="I124">
         <v>1114.2998050000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J124">
+        <v>113623993.7086636</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>3357</v>
       </c>
       <c r="B125" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D125">
         <v>626.33892800000001</v>
@@ -4167,16 +4542,19 @@
       <c r="I125">
         <v>1100.958862</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J125">
+        <v>115667993.73727059</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>3389</v>
       </c>
       <c r="B126" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D126">
         <v>832.27955498576114</v>
@@ -4196,16 +4574,19 @@
       <c r="I126">
         <v>1051.5732102106249</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J126">
+        <v>6905294.4530950673</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>3591</v>
       </c>
       <c r="B127" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C127" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D127">
         <v>619.15429700000004</v>
@@ -4225,16 +4606,19 @@
       <c r="I127">
         <v>829.02099599999997</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J127">
+        <v>12845468.493239909</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>3633</v>
       </c>
       <c r="B128" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C128" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D128">
         <v>644.84155299999998</v>
@@ -4254,16 +4638,19 @@
       <c r="I128">
         <v>1062.207764</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J128">
+        <v>200992712.0210312</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>3634</v>
       </c>
       <c r="B129" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C129" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D129">
         <v>1685.0317379999999</v>
@@ -4283,16 +4670,19 @@
       <c r="I129">
         <v>1056.11438</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J129">
+        <v>171542669.06311911</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>3655</v>
       </c>
       <c r="B130" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D130">
         <v>512.74908400000004</v>
@@ -4312,16 +4702,19 @@
       <c r="I130">
         <v>1107.0477289999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J130">
+        <v>247125115.75061259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>3661</v>
       </c>
       <c r="B131" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C131" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D131">
         <v>3564.0466310000002</v>
@@ -4341,16 +4734,19 @@
       <c r="I131">
         <v>169.67408800000001</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J131">
+        <v>120543018.34000351</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>3674</v>
       </c>
       <c r="B132" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C132" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D132">
         <v>3592.4270019999999</v>
@@ -4370,16 +4766,19 @@
       <c r="I132">
         <v>816.933899</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J132">
+        <v>11343077.455338471</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>3680</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D133">
         <v>2850.2446289999998</v>
@@ -4399,16 +4798,19 @@
       <c r="I133">
         <v>1047.9379879999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J133">
+        <v>746775051.3485837</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>3687</v>
       </c>
       <c r="B134" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D134">
         <v>2851.7460940000001</v>
@@ -4428,16 +4830,19 @@
       <c r="I134">
         <v>1044.556763</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J134">
+        <v>558414593.87999749</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>3697</v>
       </c>
       <c r="B135" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D135">
         <v>3777.7163089999999</v>
@@ -4457,16 +4862,19 @@
       <c r="I135">
         <v>813.84808299999997</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J135">
+        <v>2140993.721058113</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>3698</v>
       </c>
       <c r="B136" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D136">
         <v>168.79808</v>
@@ -4486,16 +4894,19 @@
       <c r="I136">
         <v>1108.699707</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J136">
+        <v>724877236.05331504</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>3699</v>
       </c>
       <c r="B137" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" t="s">
         <v>12</v>
-      </c>
-      <c r="C137" t="s">
-        <v>11</v>
       </c>
       <c r="D137">
         <v>2829.26001</v>
@@ -4515,16 +4926,19 @@
       <c r="I137">
         <v>1063.0943600000001</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J137">
+        <v>322736281.40574932</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>3741</v>
       </c>
       <c r="B138" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C138" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D138">
         <v>2589.0559079999998</v>
@@ -4544,16 +4958,19 @@
       <c r="I138">
         <v>867.31274399999995</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J138">
+        <v>12987533.297290999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>3775</v>
       </c>
       <c r="B139" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C139" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D139">
         <v>426.67022700000001</v>
@@ -4573,16 +4990,19 @@
       <c r="I139">
         <v>366</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J139">
+        <v>51057387.043277957</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>3787</v>
       </c>
       <c r="B140" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C140" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D140">
         <v>1857.8432620000001</v>
@@ -4602,16 +5022,19 @@
       <c r="I140">
         <v>362.86459400000001</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J140">
+        <v>74089778.389638901</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>3809</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C141" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D141">
         <v>2575.0161130000001</v>
@@ -4631,16 +5054,19 @@
       <c r="I141">
         <v>317.762787</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J141">
+        <v>83927342.146729976</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>3812</v>
       </c>
       <c r="B142" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C142" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D142">
         <v>2634.8000489999999</v>
@@ -4660,16 +5086,19 @@
       <c r="I142">
         <v>679.78851299999997</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J142">
+        <v>156249925.68286541</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>3814</v>
       </c>
       <c r="B143" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C143" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D143">
         <v>3573.4936520000001</v>
@@ -4689,16 +5118,19 @@
       <c r="I143">
         <v>354.20117199999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J143">
+        <v>19084242.942981709</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>3822</v>
       </c>
       <c r="B144" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C144" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D144">
         <v>1115.828929289524</v>
@@ -4718,16 +5150,19 @@
       <c r="I144">
         <v>1099.280550046808</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J144">
+        <v>4539732.320076854</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>3824</v>
       </c>
       <c r="B145" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C145" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D145">
         <v>359.66861</v>
@@ -4747,16 +5182,19 @@
       <c r="I145">
         <v>1048.556274</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J145">
+        <v>46744007.495347701</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>3830</v>
       </c>
       <c r="B146" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C146" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D146">
         <v>1014.387634</v>
@@ -4776,16 +5214,19 @@
       <c r="I146">
         <v>1177.623779</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J146">
+        <v>772801582.2698251</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>3849</v>
       </c>
       <c r="B147" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D147">
         <v>641</v>
@@ -4805,16 +5246,19 @@
       <c r="I147">
         <v>682.16711399999997</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J147">
+        <v>1536995.6537733199</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>3897</v>
       </c>
       <c r="B148" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D148">
         <v>1720.8496090000001</v>
@@ -4834,16 +5278,19 @@
       <c r="I148">
         <v>1066.8023679999999</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J148">
+        <v>87536796.362904146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>3918</v>
       </c>
       <c r="B149" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D149">
         <v>626.33892800000001</v>
@@ -4863,16 +5310,19 @@
       <c r="I149">
         <v>1072.5979</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J149">
+        <v>101185162.6066363</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>3934</v>
       </c>
       <c r="B150" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D150">
         <v>1055.770264</v>
@@ -4892,16 +5342,19 @@
       <c r="I150">
         <v>1193.626221</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J150">
+        <v>399961538.39839971</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>3936</v>
       </c>
       <c r="B151" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C151" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D151">
         <v>832.27955498576114</v>
@@ -4921,16 +5374,19 @@
       <c r="I151">
         <v>1051.5732102106249</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J151">
+        <v>6905294.4530950673</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>3946</v>
       </c>
       <c r="B152" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -4950,16 +5406,19 @@
       <c r="I152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>3948</v>
       </c>
       <c r="B153" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D153">
         <v>1081.74663646662</v>
@@ -4979,16 +5438,19 @@
       <c r="I153">
         <v>901.2300587420475</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>3963</v>
       </c>
       <c r="B154" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C154" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -5008,16 +5470,19 @@
       <c r="I154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>3989</v>
       </c>
       <c r="B155" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -5037,16 +5502,19 @@
       <c r="I155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>4037</v>
       </c>
       <c r="B156" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C156" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -5066,16 +5534,19 @@
       <c r="I156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>4045</v>
       </c>
       <c r="B157" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C157" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -5095,16 +5566,19 @@
       <c r="I157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>4054</v>
       </c>
       <c r="B158" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C158" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -5124,16 +5598,19 @@
       <c r="I158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>4086</v>
       </c>
       <c r="B159" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C159" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D159">
         <v>2206.2994560776078</v>
@@ -5153,16 +5630,19 @@
       <c r="I159">
         <v>948.0421270015089</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J159">
+        <v>3007265.5118336622</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>4087</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D160">
         <v>2210.407331506326</v>
@@ -5182,16 +5662,19 @@
       <c r="I160">
         <v>938.70272756775455</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J160">
+        <v>2709722.554991364</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>4088</v>
       </c>
       <c r="B161" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C161" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D161">
         <v>2892.423290698001</v>
@@ -5211,16 +5694,19 @@
       <c r="I161">
         <v>1143.162805065248</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J161">
+        <v>512050.74384261732</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>4089</v>
       </c>
       <c r="B162" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C162" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D162">
         <v>2939.6213184558069</v>
@@ -5240,16 +5726,19 @@
       <c r="I162">
         <v>1163.7556454087321</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J162">
+        <v>748721.45857866819</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>4090</v>
       </c>
       <c r="B163" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C163" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D163">
         <v>2229.6801087981939</v>
@@ -5269,16 +5758,19 @@
       <c r="I163">
         <v>1124.6196850445849</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J163">
+        <v>1757254.837009503</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>4091</v>
       </c>
       <c r="B164" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D164">
         <v>2215.891416094405</v>
@@ -5298,16 +5790,19 @@
       <c r="I164">
         <v>1121.059575566441</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J164">
+        <v>1742094.473237742</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>4092</v>
       </c>
       <c r="B165" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C165" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D165">
         <v>1374.489003575593</v>
@@ -5326,6 +5821,9 @@
       </c>
       <c r="I165">
         <v>1211.4026482057229</v>
+      </c>
+      <c r="J165">
+        <v>1618661.12250096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>